<commit_message>
add displaayName and descrption of Property's property
</commit_message>
<xml_diff>
--- a/Excel2DTDL/Excel2DTDL_Template.xlsx
+++ b/Excel2DTDL/Excel2DTDL_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iloh\source\excel2dtdl\Excel2DTDL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380BB404-1F1E-4877-9996-97427725BBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE8FDC4-68B0-40C4-887E-9FB3ACD347B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16590" yWindow="3705" windowWidth="38700" windowHeight="14925" activeTab="1" xr2:uid="{B1ED5F9A-0777-495C-B70C-3BD137737F8F}"/>
+    <workbookView xWindow="23985" yWindow="3000" windowWidth="22545" windowHeight="17460" activeTab="1" xr2:uid="{B1ED5F9A-0777-495C-B70C-3BD137737F8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Factory" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="68">
   <si>
     <t>name</t>
   </si>
@@ -224,6 +224,24 @@
   </si>
   <si>
     <t>Temperature1</t>
+  </si>
+  <si>
+    <t>FloodId 입니다.</t>
+  </si>
+  <si>
+    <t>Floor ID</t>
+  </si>
+  <si>
+    <t>Floor Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Floor Name 입니다. </t>
+  </si>
+  <si>
+    <t>층온도</t>
+  </si>
+  <si>
+    <t>층온도 평균값</t>
   </si>
 </sst>
 </file>
@@ -289,7 +307,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="88">
+  <dxfs count="90">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -568,196 +592,198 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7A1024B5-1E50-453E-915B-3B64E3A6A38C}" name="Table214" displayName="Table214" ref="B3:F8" totalsRowShown="0" headerRowDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7A1024B5-1E50-453E-915B-3B64E3A6A38C}" name="Table214" displayName="Table214" ref="B3:F8" totalsRowShown="0" headerRowDxfId="89">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{744A1E34-3894-4D92-B81A-9B867114D95F}" name="name" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{1A3518E1-BA5B-4AFA-860D-EDF646AE7380}" name="schema" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{A5FD6ABC-7124-4B97-98C6-9BEE5BA00043}" name="writable?" dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{0AAC6286-90B7-4E53-B21C-B2ADB37BE01D}" name="type?" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{52CD93BB-EFEE-45E8-9999-7F4E7E7438E8}" name="unit?" dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{744A1E34-3894-4D92-B81A-9B867114D95F}" name="name" dataDxfId="88"/>
+    <tableColumn id="2" xr3:uid="{1A3518E1-BA5B-4AFA-860D-EDF646AE7380}" name="schema" dataDxfId="87"/>
+    <tableColumn id="3" xr3:uid="{A5FD6ABC-7124-4B97-98C6-9BEE5BA00043}" name="writable?" dataDxfId="86"/>
+    <tableColumn id="4" xr3:uid="{0AAC6286-90B7-4E53-B21C-B2ADB37BE01D}" name="type?" dataDxfId="85"/>
+    <tableColumn id="5" xr3:uid="{52CD93BB-EFEE-45E8-9999-7F4E7E7438E8}" name="unit?" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{81079CA0-5562-4454-A683-1DFB19C603A1}" name="Table28" displayName="Table28" ref="B3:F7" totalsRowShown="0" headerRowDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{81079CA0-5562-4454-A683-1DFB19C603A1}" name="Table28" displayName="Table28" ref="B3:F7" totalsRowShown="0" headerRowDxfId="36">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F8C9ECA1-7A85-4311-B66C-6D2320F5CC3A}" name="name" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{752E85D2-2138-4517-9AA3-A2D7D28515BE}" name="schema" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{8FDE5A14-454C-46FA-9FB9-C61BC4693F75}" name="writable?" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{F9881EC1-FD17-423A-9FA0-FADE48DBF922}" name="type?" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{A6F477A8-4853-44DB-8470-8537EBFE4A81}" name="unit?" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{F8C9ECA1-7A85-4311-B66C-6D2320F5CC3A}" name="name" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{752E85D2-2138-4517-9AA3-A2D7D28515BE}" name="schema" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{8FDE5A14-454C-46FA-9FB9-C61BC4693F75}" name="writable?" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{F9881EC1-FD17-423A-9FA0-FADE48DBF922}" name="type?" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{A6F477A8-4853-44DB-8470-8537EBFE4A81}" name="unit?" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{0C80EE20-5C7C-4419-9FEA-F5C274AC68CD}" name="Table511" displayName="Table511" ref="B8:D11" totalsRowShown="0" headerRowDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{0C80EE20-5C7C-4419-9FEA-F5C274AC68CD}" name="Table511" displayName="Table511" ref="B8:D11" totalsRowShown="0" headerRowDxfId="30">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E4B36B03-966D-49EE-9798-D823BA4989A0}" name="name" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{022B714C-C911-4A27-AB6B-C5BB5405D64C}" name="displayName?" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{EDF8451D-651E-4633-A313-4B19888EDE3B}" name="target" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{E4B36B03-966D-49EE-9798-D823BA4989A0}" name="name" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{022B714C-C911-4A27-AB6B-C5BB5405D64C}" name="displayName?" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{EDF8451D-651E-4633-A313-4B19888EDE3B}" name="target" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8DB1BCE7-0A0B-43FD-8208-1232CB6EDA5B}" name="Table2" displayName="Table2" ref="B3:F7" totalsRowShown="0" headerRowDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8DB1BCE7-0A0B-43FD-8208-1232CB6EDA5B}" name="Table2" displayName="Table2" ref="B3:F7" totalsRowShown="0" headerRowDxfId="26">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{15FD9AA7-9D26-4C83-B854-C4BA7A290DAD}" name="name" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{A8957FCD-08D0-43BC-BC1A-9FA20DFCB081}" name="schema" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{A58E18E6-3927-4319-AFF5-072562A88800}" name="writable?" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{B71323B9-5465-455E-87E1-F7F16D63ADB2}" name="type?" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{1C95DAA0-40A1-42A1-9487-B06DC380E5E8}" name="unit?" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{15FD9AA7-9D26-4C83-B854-C4BA7A290DAD}" name="name" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{A8957FCD-08D0-43BC-BC1A-9FA20DFCB081}" name="schema" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{A58E18E6-3927-4319-AFF5-072562A88800}" name="writable?" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{B71323B9-5465-455E-87E1-F7F16D63ADB2}" name="type?" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{1C95DAA0-40A1-42A1-9487-B06DC380E5E8}" name="unit?" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5B445B8F-59AC-45BE-A547-CE8FB85900DE}" name="Table3" displayName="Table3" ref="B8:E10" totalsRowShown="0" headerRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5B445B8F-59AC-45BE-A547-CE8FB85900DE}" name="Table3" displayName="Table3" ref="B8:E10" totalsRowShown="0" headerRowDxfId="20">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{1095416C-3108-434F-98AE-0BBA6982D530}" name="name" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{AEF7F29C-E0AC-44F4-9136-8E60BD3C7E9D}" name="schema" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{6D856199-FB48-4C8D-AAA0-CE3DCAF1095B}" name="type?" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{291922CB-ED99-46B1-83AA-8A07506EF185}" name="unit?" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{1095416C-3108-434F-98AE-0BBA6982D530}" name="name" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{AEF7F29C-E0AC-44F4-9136-8E60BD3C7E9D}" name="schema" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{6D856199-FB48-4C8D-AAA0-CE3DCAF1095B}" name="type?" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{291922CB-ED99-46B1-83AA-8A07506EF185}" name="unit?" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F71CBBCB-F4B4-4A71-90AA-C0E8DD1A5D7D}" name="Table4" displayName="Table4" ref="B11:E12" totalsRowShown="0" headerRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F71CBBCB-F4B4-4A71-90AA-C0E8DD1A5D7D}" name="Table4" displayName="Table4" ref="B11:E12" totalsRowShown="0" headerRowDxfId="15">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E44DCDF6-EF82-4076-B06B-76BBA748275C}" name="name" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{4515CC3B-EFDB-49FF-8926-35C417DF3B71}" name="schema" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{6B6D4A74-6606-457B-A34A-9A6194171B42}" name="displayName?" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{AB46E9E0-E004-4EBE-84B8-C363EFF814E8}" name="description?" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{E44DCDF6-EF82-4076-B06B-76BBA748275C}" name="name" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{4515CC3B-EFDB-49FF-8926-35C417DF3B71}" name="schema" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{6B6D4A74-6606-457B-A34A-9A6194171B42}" name="displayName?" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{AB46E9E0-E004-4EBE-84B8-C363EFF814E8}" name="description?" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B91BE8ED-BB3B-403E-B96F-7B061151545E}" name="Table5" displayName="Table5" ref="B13:D14" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B91BE8ED-BB3B-403E-B96F-7B061151545E}" name="Table5" displayName="Table5" ref="B13:D14" totalsRowShown="0" headerRowDxfId="10">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9CD63EC7-BF65-4001-B18E-E0FE6AAEAA55}" name="name" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{AD9EEE65-C8DA-498B-A2FC-2680B307891D}" name="displayName?" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{62A5F339-6D60-48BC-A9C5-FED29A45BED3}" name="target" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{9CD63EC7-BF65-4001-B18E-E0FE6AAEAA55}" name="name" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{AD9EEE65-C8DA-498B-A2FC-2680B307891D}" name="displayName?" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{62A5F339-6D60-48BC-A9C5-FED29A45BED3}" name="target" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{1EF3180D-282F-4450-B29F-A71080E1440D}" name="Table1710" displayName="Table1710" ref="B1:F2" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{1EF3180D-282F-4450-B29F-A71080E1440D}" name="Table1710" displayName="Table1710" ref="B1:F2" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7F9A35F7-F27B-4057-BC58-F162D9AA0DF1}" name="id" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{EFA8F779-6354-4BAA-B22B-20DFE8745F92}" name="name" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{DC01178C-8827-4EE6-B033-ABE396027C8C}" name="displayName" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{233FED2F-0F32-49E7-9505-E7825C91459D}" name="extends?" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{419FF7F4-CBE6-458D-B42B-FAD35C44CD5E}" name="description?" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{7F9A35F7-F27B-4057-BC58-F162D9AA0DF1}" name="id" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{EFA8F779-6354-4BAA-B22B-20DFE8745F92}" name="name" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{DC01178C-8827-4EE6-B033-ABE396027C8C}" name="displayName" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{233FED2F-0F32-49E7-9505-E7825C91459D}" name="extends?" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{419FF7F4-CBE6-458D-B42B-FAD35C44CD5E}" name="description?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{AE55B30B-A2D3-45F4-81E9-76910F8EA8F6}" name="Table517" displayName="Table517" ref="B9:D11" totalsRowShown="0" headerRowDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{AE55B30B-A2D3-45F4-81E9-76910F8EA8F6}" name="Table517" displayName="Table517" ref="B9:D11" totalsRowShown="0" headerRowDxfId="83">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{F2A011C8-CADE-4B33-A9F3-01D64E19EE93}" name="name" dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{6232EAAA-093F-490F-ADB0-DE6BB1E49753}" name="displayName?" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{55E5755B-C84F-43CD-B31A-183C944477A8}" name="target" dataDxfId="52"/>
+    <tableColumn id="1" xr3:uid="{F2A011C8-CADE-4B33-A9F3-01D64E19EE93}" name="name" dataDxfId="82"/>
+    <tableColumn id="2" xr3:uid="{6232EAAA-093F-490F-ADB0-DE6BB1E49753}" name="displayName?" dataDxfId="81"/>
+    <tableColumn id="3" xr3:uid="{55E5755B-C84F-43CD-B31A-183C944477A8}" name="target" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{E466D8F3-7547-497C-BD65-C24A6903A25E}" name="Table113" displayName="Table113" ref="B1:F2" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{E466D8F3-7547-497C-BD65-C24A6903A25E}" name="Table113" displayName="Table113" ref="B1:F2" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C8A45F92-1065-4BA7-97CF-C4E78081379A}" name="id" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{6AD01C16-DC59-4B43-A36D-B5A8E890A40F}" name="name" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{E51D4CA9-FCDE-4CD5-9D1E-48B29B7153FE}" name="displayName2" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{AB6689FB-4C32-4E5B-BFBD-FDBBCCD0F456}" name="extends" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{5FFB323D-7639-4E0B-AEB1-50D3D4E8C2C1}" name="description" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{C8A45F92-1065-4BA7-97CF-C4E78081379A}" name="id" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{6AD01C16-DC59-4B43-A36D-B5A8E890A40F}" name="name" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{E51D4CA9-FCDE-4CD5-9D1E-48B29B7153FE}" name="displayName2" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{AB6689FB-4C32-4E5B-BFBD-FDBBCCD0F456}" name="extends" dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{5FFB323D-7639-4E0B-AEB1-50D3D4E8C2C1}" name="description" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BB43936B-53A5-4DC5-A177-064305A3A015}" name="Table22" displayName="Table22" ref="B3:F7" totalsRowShown="0" headerRowDxfId="87">
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7DD405C8-A20E-4A53-B871-2D0B3704EA58}" name="name" dataDxfId="86"/>
-    <tableColumn id="2" xr3:uid="{852F8340-B7B1-46C0-874B-59B7E629A914}" name="schema" dataDxfId="85"/>
-    <tableColumn id="3" xr3:uid="{00E8A1E8-C183-4AF7-B57C-5D47858897BC}" name="writable?" dataDxfId="84"/>
-    <tableColumn id="4" xr3:uid="{14D38BDD-5681-4E9C-BE33-B59FF4CF9403}" name="type?" dataDxfId="83"/>
-    <tableColumn id="5" xr3:uid="{A1927546-07B8-46D9-A662-2FE6238FDAB0}" name="unit?" dataDxfId="82"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BB43936B-53A5-4DC5-A177-064305A3A015}" name="Table22" displayName="Table22" ref="B3:H7" totalsRowShown="0" headerRowDxfId="72">
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{7DD405C8-A20E-4A53-B871-2D0B3704EA58}" name="name" dataDxfId="71"/>
+    <tableColumn id="2" xr3:uid="{852F8340-B7B1-46C0-874B-59B7E629A914}" name="schema" dataDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{00E8A1E8-C183-4AF7-B57C-5D47858897BC}" name="writable?" dataDxfId="69"/>
+    <tableColumn id="4" xr3:uid="{14D38BDD-5681-4E9C-BE33-B59FF4CF9403}" name="type?" dataDxfId="68"/>
+    <tableColumn id="5" xr3:uid="{A1927546-07B8-46D9-A662-2FE6238FDAB0}" name="unit?" dataDxfId="67"/>
+    <tableColumn id="6" xr3:uid="{39E05725-E676-412A-B8DC-42A830D2A312}" name="displayName" dataDxfId="66"/>
+    <tableColumn id="7" xr3:uid="{8A335C78-B5BC-4F67-8A9E-71549DC9703E}" name="description" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A16383E3-41FE-42BE-93EE-0B5D88CB8142}" name="Table39" displayName="Table39" ref="B8:E10" totalsRowShown="0" headerRowDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A16383E3-41FE-42BE-93EE-0B5D88CB8142}" name="Table39" displayName="Table39" ref="B8:E10" totalsRowShown="0" headerRowDxfId="64">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{54B2D2A0-C81C-48DC-8132-C3F505031D8E}" name="name" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{AFB6F5A0-50C3-40D7-ADFA-42D6706A1BD7}" name="schema" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{F3181107-9E62-43A0-8FCB-6FEE8486B44B}" name="type?" dataDxfId="78"/>
-    <tableColumn id="4" xr3:uid="{3F96E644-4BCA-4FBE-B2AB-E98065632338}" name="unit?" dataDxfId="77"/>
+    <tableColumn id="1" xr3:uid="{54B2D2A0-C81C-48DC-8132-C3F505031D8E}" name="name" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{AFB6F5A0-50C3-40D7-ADFA-42D6706A1BD7}" name="schema" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{F3181107-9E62-43A0-8FCB-6FEE8486B44B}" name="type?" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{3F96E644-4BCA-4FBE-B2AB-E98065632338}" name="unit?" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{E7EFFC6F-804E-4E17-A56F-AB22B3C0D54B}" name="Table412" displayName="Table412" ref="B11:E12" totalsRowShown="0" headerRowDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{E7EFFC6F-804E-4E17-A56F-AB22B3C0D54B}" name="Table412" displayName="Table412" ref="B11:E12" totalsRowShown="0" headerRowDxfId="59">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3376823B-2272-4388-852E-A4145B7653D9}" name="name" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{AC798E63-6B40-44CF-B923-76966C44ECF7}" name="schema" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{1E3D7BA6-1E80-46EF-96B6-D8C16221AF3D}" name="displayName?" dataDxfId="74"/>
-    <tableColumn id="4" xr3:uid="{BC6F69FC-E8FD-428D-B36D-C14D4D3BF3B1}" name="description?" dataDxfId="73"/>
+    <tableColumn id="1" xr3:uid="{3376823B-2272-4388-852E-A4145B7653D9}" name="name" dataDxfId="58"/>
+    <tableColumn id="2" xr3:uid="{AC798E63-6B40-44CF-B923-76966C44ECF7}" name="schema" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{1E3D7BA6-1E80-46EF-96B6-D8C16221AF3D}" name="displayName?" dataDxfId="56"/>
+    <tableColumn id="4" xr3:uid="{BC6F69FC-E8FD-428D-B36D-C14D4D3BF3B1}" name="description?" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{386F1C9F-32DD-46C6-A957-772CA6EA17CD}" name="Table515" displayName="Table515" ref="B13:D14" totalsRowShown="0" headerRowDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{386F1C9F-32DD-46C6-A957-772CA6EA17CD}" name="Table515" displayName="Table515" ref="B13:D14" totalsRowShown="0" headerRowDxfId="54">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{C18503A1-B979-46A3-A29A-E107F0E66418}" name="name" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{C521ECA7-5F03-4A89-A9C4-80D4C36785BD}" name="displayName?" dataDxfId="70"/>
-    <tableColumn id="3" xr3:uid="{C8E1C223-2D00-41AB-9AA4-6C1CE2B7DA61}" name="target" dataDxfId="69"/>
+    <tableColumn id="1" xr3:uid="{C18503A1-B979-46A3-A29A-E107F0E66418}" name="name" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{C521ECA7-5F03-4A89-A9C4-80D4C36785BD}" name="displayName?" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{C8E1C223-2D00-41AB-9AA4-6C1CE2B7DA61}" name="target" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{DE5760EC-6228-4C2D-9E4C-0EBA8A282DA9}" name="Table171016" displayName="Table171016" ref="B1:F2" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{DE5760EC-6228-4C2D-9E4C-0EBA8A282DA9}" name="Table171016" displayName="Table171016" ref="B1:F2" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A2ADA601-95B6-40A7-816E-05FA0352B8AE}" name="id" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{7D6F9AB8-E186-4420-A5D1-CBD2B87D5D12}" name="name" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{1269729A-1F81-4EFC-BF31-C04406E0884D}" name="displayName" dataDxfId="64"/>
-    <tableColumn id="4" xr3:uid="{8749182D-6FE9-4049-8506-18FC27F3930D}" name="extends?" dataDxfId="63"/>
-    <tableColumn id="6" xr3:uid="{F2A4373A-5E64-4E85-9EC7-1F900D657B54}" name="description?" dataDxfId="62"/>
+    <tableColumn id="1" xr3:uid="{A2ADA601-95B6-40A7-816E-05FA0352B8AE}" name="id" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{7D6F9AB8-E186-4420-A5D1-CBD2B87D5D12}" name="name" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{1269729A-1F81-4EFC-BF31-C04406E0884D}" name="displayName" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{8749182D-6FE9-4049-8506-18FC27F3930D}" name="extends?" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{F2A4373A-5E64-4E85-9EC7-1F900D657B54}" name="description?" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{794E2690-DA4B-4FBA-90A1-328FACE5663F}" name="Table17" displayName="Table17" ref="B1:F2" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{794E2690-DA4B-4FBA-90A1-328FACE5663F}" name="Table17" displayName="Table17" ref="B1:F2" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{CC8CC584-DC9E-453C-BAAA-03D1D980276A}" name="id" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{A2534418-A90A-49FA-BC76-F6B328808FA9}" name="name" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{562AB957-4C59-4F9D-80AB-F5FD992CAB7F}" name="displayName" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{FD802B25-1643-45A9-B4DC-07E89BF691E9}" name="extends" dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{9C5E9F5A-0388-4386-B3D0-FF2C29A92A1D}" name="description" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{CC8CC584-DC9E-453C-BAAA-03D1D980276A}" name="id" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{A2534418-A90A-49FA-BC76-F6B328808FA9}" name="name" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{562AB957-4C59-4F9D-80AB-F5FD992CAB7F}" name="displayName" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{FD802B25-1643-45A9-B4DC-07E89BF691E9}" name="extends" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{9C5E9F5A-0388-4386-B3D0-FF2C29A92A1D}" name="description" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1224,10 +1250,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C304BF10-89C2-4430-9C4E-1F7D857D12D5}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1238,10 +1264,12 @@
     <col min="4" max="4" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.28515625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
+    <col min="7" max="7" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -1261,7 +1289,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>59</v>
       </c>
@@ -1272,7 +1300,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
@@ -1291,8 +1319,14 @@
       <c r="F3" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
@@ -1302,8 +1336,14 @@
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1313,8 +1353,14 @@
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1330,8 +1376,14 @@
       <c r="F6" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
@@ -1339,7 +1391,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1356,7 +1408,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>61</v>
       </c>
@@ -1370,7 +1422,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
@@ -1378,7 +1430,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1395,7 +1447,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>51</v>
       </c>
@@ -1403,7 +1455,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -1417,7 +1469,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>